<commit_message>
Pruebas funcionales TC 003 Alcosto
</commit_message>
<xml_diff>
--- a/Alkosto/Pruebas Funcionales/AlkostoDataDrive.xlsx
+++ b/Alkosto/Pruebas Funcionales/AlkostoDataDrive.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FuentesTFS\eafit.verificacionValidacion\Alkosto\Pruebas Funcionales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF849758-A0D8-4F72-9C07-887E53695C42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675E8FB4-3CE7-473F-900D-884BA85D26EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{D95ABBBB-F731-4F59-898C-B4B9AAA53186}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{D95ABBBB-F731-4F59-898C-B4B9AAA53186}"/>
   </bookViews>
   <sheets>
     <sheet name="Data001" sheetId="1" r:id="rId1"/>
     <sheet name="Data002" sheetId="2" r:id="rId2"/>
+    <sheet name="Data003" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>producto</t>
   </si>
@@ -52,6 +53,12 @@
   </si>
   <si>
     <t>LG</t>
+  </si>
+  <si>
+    <t>busqueda</t>
+  </si>
+  <si>
+    <t>Portatil Lenovo</t>
   </si>
 </sst>
 </file>
@@ -445,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2254C073-98B4-4748-B3F8-8E25F8089473}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,4 +492,32 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE6C21E-95E1-4EF8-89CD-FEF92871604D}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>